<commit_message>
suppression de code inutile
</commit_message>
<xml_diff>
--- a/FinFolio/FinFolio/FinFolio-feature_Gestion_User/finfolio2/Depense2.xlsx
+++ b/FinFolio/FinFolio/FinFolio-feature_Gestion_User/finfolio2/Depense2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -32,13 +32,40 @@
     <t>User</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>2024-04-05</t>
-  </si>
-  <si>
-    <t>jkk</t>
+    <t>hdhd</t>
+  </si>
+  <si>
+    <t>2024-03-16</t>
+  </si>
+  <si>
+    <t>ffjff</t>
+  </si>
+  <si>
+    <t>nourriture</t>
+  </si>
+  <si>
+    <t>2024-03-23</t>
+  </si>
+  <si>
+    <t>hljnjf</t>
+  </si>
+  <si>
+    <t>jjdjdd</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>try44</t>
+  </si>
+  <si>
+    <t>2024-03-30</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>tryyyy</t>
   </si>
 </sst>
 </file>
@@ -83,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -111,7 +138,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>234.0</v>
+        <v>269.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>6</v>
@@ -120,10 +147,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>456.0</v>
+        <v>785.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>63.84000015258789</v>
+        <v>109.9000015258789</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>106.0</v>
@@ -131,7 +158,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>227.0</v>
+        <v>273.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>8</v>
@@ -140,12 +167,132 @@
         <v>7</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>886.0</v>
+        <v>755598.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>124.04000091552734</v>
+        <v>105784.0</v>
       </c>
       <c r="F3" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>259.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>272.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>5555.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>777.7000122070312</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>266.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>48748.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>6824.72021484375</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>264.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>456.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>63.84000015258789</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>274.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>456.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>63.84000015258789</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>275.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>5455.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>763.7000122070312</v>
+      </c>
+      <c r="F9" t="n" s="0">
         <v>106.0</v>
       </c>
     </row>

</xml_diff>